<commit_message>
Ignore MS Office "Is Open" flag files
</commit_message>
<xml_diff>
--- a/api/_admin/Prefixes_Suffixes.xlsx
+++ b/api/_admin/Prefixes_Suffixes.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="44">
   <si>
     <t>prefix</t>
   </si>
@@ -121,6 +121,33 @@
   </si>
   <si>
     <t>Geometry - Polygon</t>
+  </si>
+  <si>
+    <t>Helper Graphics/PostGIS tables</t>
+  </si>
+  <si>
+    <t>keyword</t>
+  </si>
+  <si>
+    <t>Count of requested attributes</t>
+  </si>
+  <si>
+    <t>Requested attributes, e.g. bn=2&amp;b0=hi&amp;b1=there</t>
+  </si>
+  <si>
+    <t>dn</t>
+  </si>
+  <si>
+    <t>d[0-9]+</t>
+  </si>
+  <si>
+    <t>Data request</t>
+  </si>
+  <si>
+    <t>Identifier request</t>
+  </si>
+  <si>
+    <t>Geometry request</t>
   </si>
 </sst>
 </file>
@@ -459,208 +486,268 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N16" sqref="N16"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>22</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>23</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>8</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>30</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>7</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>10</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
         <v>4</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>7</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>10</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
         <v>5</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>7</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>10</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
         <v>6</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>7</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>10</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G6" t="s">
+        <v>10</v>
+      </c>
+      <c r="I6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
         <v>11</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E7" t="s">
         <v>7</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G7" t="s">
         <v>12</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
         <v>24</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D8" t="s">
         <v>11</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E8" t="s">
         <v>7</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G8" t="s">
         <v>12</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I8" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>14</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E9" t="s">
         <v>13</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G9" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="I9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>15</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E10" t="s">
         <v>13</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G10" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="I10" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>39</v>
+      </c>
+      <c r="E11" t="s">
+        <v>13</v>
+      </c>
+      <c r="F11" t="s">
+        <v>15</v>
+      </c>
+      <c r="G11" t="s">
+        <v>17</v>
+      </c>
+      <c r="I11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>40</v>
+      </c>
+      <c r="E12" t="s">
+        <v>13</v>
+      </c>
+      <c r="F12" t="s">
+        <v>15</v>
+      </c>
+      <c r="G12" t="s">
+        <v>17</v>
+      </c>
+      <c r="I12" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>16</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E13" t="s">
         <v>13</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G13" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="I13" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>27</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E14" t="s">
         <v>13</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G14" t="s">
         <v>17</v>
       </c>
-      <c r="G11" t="s">
+      <c r="H14" t="s">
         <v>31</v>
       </c>
-      <c r="H11" t="s">
+      <c r="I14" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>28</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E15" t="s">
         <v>13</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G15" t="s">
         <v>17</v>
       </c>
-      <c r="G12" t="s">
+      <c r="H15" t="s">
         <v>31</v>
       </c>
-      <c r="H12" t="s">
+      <c r="I15" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>29</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E16" t="s">
         <v>13</v>
       </c>
-      <c r="F13" t="s">
+      <c r="G16" t="s">
         <v>17</v>
       </c>
-      <c r="G13" t="s">
+      <c r="H16" t="s">
         <v>31</v>
       </c>
-      <c r="H13" t="s">
+      <c r="I16" t="s">
         <v>34</v>
       </c>
     </row>

</xml_diff>